<commit_message>
minimos cuadrados con pesos
</commit_message>
<xml_diff>
--- a/2. Magnetostricción/Code/Caracterizacion.xlsx
+++ b/2. Magnetostricción/Code/Caracterizacion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Intermedio\Intrr\Intermedio\2. Magnetostricción\Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\Documents\GitHub\Intermedio\2. Magnetostricción\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B12E8520-6F17-4CB8-8AC1-D8D69A4C79BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7020A750-21EB-4E18-A0DB-B796DA3FDA8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{C24F83B0-B571-417A-8C55-2A28262D387B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C24F83B0-B571-417A-8C55-2A28262D387B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Corriente (A)</t>
   </si>
   <si>
-    <t>Campo Magnético (T)</t>
+    <t>Campo Magnético (mT)</t>
+  </si>
+  <si>
+    <t>error_corriente (A)</t>
+  </si>
+  <si>
+    <t>error_campo (mT)</t>
   </si>
 </sst>
 </file>
@@ -413,484 +419,843 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E317FCE5-E4DA-4306-9379-595E0BA0B1CE}">
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>-2.88</v>
       </c>
       <c r="B2">
         <v>-54.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>0.01</v>
+      </c>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>-2.77</v>
       </c>
       <c r="B3">
         <v>-51.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>0.01</v>
+      </c>
+      <c r="D3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>-2.67</v>
       </c>
       <c r="B4">
         <v>-49.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>0.01</v>
+      </c>
+      <c r="D4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>-2.56</v>
       </c>
       <c r="B5">
         <v>-47.8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>0.01</v>
+      </c>
+      <c r="D5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>-2.48</v>
       </c>
       <c r="B6">
         <v>-45.7</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>0.01</v>
+      </c>
+      <c r="D6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>-2.37</v>
       </c>
       <c r="B7">
         <v>-44.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>0.01</v>
+      </c>
+      <c r="D7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>-2.27</v>
       </c>
       <c r="B8">
         <v>-42.9</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>0.01</v>
+      </c>
+      <c r="D8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>-2.1800000000000002</v>
       </c>
       <c r="B9">
         <v>-40.799999999999997</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>0.01</v>
+      </c>
+      <c r="D9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>-2.0699999999999998</v>
       </c>
       <c r="B10">
         <v>-38.200000000000003</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>0.01</v>
+      </c>
+      <c r="D10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>-1.96</v>
       </c>
       <c r="B11">
         <v>-37.299999999999997</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>0.01</v>
+      </c>
+      <c r="D11">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>-1.87</v>
       </c>
       <c r="B12">
         <v>-34.799999999999997</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>0.01</v>
+      </c>
+      <c r="D12">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>-1.77</v>
       </c>
       <c r="B13">
         <v>-32.4</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>0.01</v>
+      </c>
+      <c r="D13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>-1.67</v>
       </c>
       <c r="B14">
         <v>-30.8</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>0.01</v>
+      </c>
+      <c r="D14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>-1.57</v>
       </c>
       <c r="B15">
         <v>-29.8</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>0.01</v>
+      </c>
+      <c r="D15">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>-1.46</v>
       </c>
       <c r="B16">
         <v>-26.8</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>0.01</v>
+      </c>
+      <c r="D16">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>-1.37</v>
       </c>
       <c r="B17">
         <v>-25.3</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>0.01</v>
+      </c>
+      <c r="D17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>-1.26</v>
       </c>
       <c r="B18">
         <v>-24.2</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>0.01</v>
+      </c>
+      <c r="D18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>-1.18</v>
       </c>
       <c r="B19">
         <v>-22.7</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>0.01</v>
+      </c>
+      <c r="D19">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>-1.07</v>
       </c>
       <c r="B20">
         <v>-19.7</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>0.01</v>
+      </c>
+      <c r="D20">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>-0.98</v>
       </c>
       <c r="B21">
         <v>-18.899999999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>0.01</v>
+      </c>
+      <c r="D21">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>-0.87</v>
       </c>
       <c r="B22">
         <v>-16.3</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>0.01</v>
+      </c>
+      <c r="D22">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>-0.78</v>
       </c>
       <c r="B23">
         <v>-14.9</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>0.01</v>
+      </c>
+      <c r="D23">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>-0.66</v>
       </c>
       <c r="B24">
         <v>-12.8</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>0.01</v>
+      </c>
+      <c r="D24">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>-0.56999999999999995</v>
       </c>
       <c r="B25">
         <v>-10.9</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>0.01</v>
+      </c>
+      <c r="D25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>-0.48</v>
       </c>
       <c r="B26">
         <v>-9.4</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>0.01</v>
+      </c>
+      <c r="D26">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>-0.36</v>
       </c>
       <c r="B27">
         <v>-7.2</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>0.01</v>
+      </c>
+      <c r="D27">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>-0.27</v>
       </c>
       <c r="B28">
         <v>-5.6</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>0.01</v>
+      </c>
+      <c r="D28">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>-0.14000000000000001</v>
       </c>
       <c r="B29">
         <v>-2.8</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>0.01</v>
+      </c>
+      <c r="D29">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>0.17</v>
       </c>
       <c r="B30">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>0.01</v>
+      </c>
+      <c r="D30">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0.27</v>
       </c>
       <c r="B31">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>0.01</v>
+      </c>
+      <c r="D31">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>0.39</v>
       </c>
       <c r="B32">
         <v>6.8</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>0.01</v>
+      </c>
+      <c r="D32">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>0.47</v>
       </c>
       <c r="B33">
         <v>8.1999999999999993</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>0.01</v>
+      </c>
+      <c r="D33">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>0.57999999999999996</v>
       </c>
       <c r="B34">
         <v>11.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>0.01</v>
+      </c>
+      <c r="D34">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>0.68</v>
       </c>
       <c r="B35">
         <v>12.3</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>0.01</v>
+      </c>
+      <c r="D35">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>0.78</v>
       </c>
       <c r="B36">
         <v>14.4</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>0.01</v>
+      </c>
+      <c r="D36">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>0.87</v>
       </c>
       <c r="B37">
         <v>15.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>0.01</v>
+      </c>
+      <c r="D37">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>0.96</v>
       </c>
       <c r="B38">
         <v>17.600000000000001</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>0.01</v>
+      </c>
+      <c r="D38">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1.08</v>
       </c>
       <c r="B39">
         <v>20.7</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>0.01</v>
+      </c>
+      <c r="D39">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1.17</v>
       </c>
       <c r="B40">
         <v>21.1</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>0.01</v>
+      </c>
+      <c r="D40">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1.28</v>
       </c>
       <c r="B41">
         <v>24.2</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>0.01</v>
+      </c>
+      <c r="D41">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1.37</v>
       </c>
       <c r="B42">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>0.01</v>
+      </c>
+      <c r="D42">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>1.47</v>
       </c>
       <c r="B43">
         <v>26.6</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>0.01</v>
+      </c>
+      <c r="D43">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1.57</v>
       </c>
       <c r="B44">
         <v>29.7</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>0.01</v>
+      </c>
+      <c r="D44">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1.67</v>
       </c>
       <c r="B45">
         <v>30.5</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>0.01</v>
+      </c>
+      <c r="D45">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1.77</v>
       </c>
       <c r="B46">
         <v>31.7</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>0.01</v>
+      </c>
+      <c r="D46">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>1.88</v>
       </c>
       <c r="B47">
         <v>35.299999999999997</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>0.01</v>
+      </c>
+      <c r="D47">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1.97</v>
       </c>
       <c r="B48">
         <v>36.200000000000003</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>0.01</v>
+      </c>
+      <c r="D48">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2.06</v>
       </c>
       <c r="B49">
         <v>38.299999999999997</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>0.01</v>
+      </c>
+      <c r="D49">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2.17</v>
       </c>
       <c r="B50">
         <v>39</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>0.01</v>
+      </c>
+      <c r="D50">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2.27</v>
       </c>
       <c r="B51">
         <v>42.8</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>0.01</v>
+      </c>
+      <c r="D51">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2.37</v>
       </c>
       <c r="B52">
         <v>43.8</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>0.01</v>
+      </c>
+      <c r="D52">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2.4700000000000002</v>
       </c>
       <c r="B53">
         <v>46.4</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>0.01</v>
+      </c>
+      <c r="D53">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2.57</v>
       </c>
       <c r="B54">
         <v>47.8</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <v>0.01</v>
+      </c>
+      <c r="D54">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2.67</v>
       </c>
       <c r="B55">
         <v>50</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>0.01</v>
+      </c>
+      <c r="D55">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2.76</v>
       </c>
       <c r="B56">
         <v>51.9</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>0.01</v>
+      </c>
+      <c r="D56">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2.89</v>
       </c>
       <c r="B57">
         <v>52.2</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>0.01</v>
+      </c>
+      <c r="D57">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2.97</v>
       </c>
       <c r="B58">
         <v>53.8</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>0.01</v>
+      </c>
+      <c r="D58">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>3.09</v>
       </c>
       <c r="B59">
         <v>57.1</v>
+      </c>
+      <c r="C59">
+        <v>0.01</v>
+      </c>
+      <c r="D59">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>